<commit_message>
Version 3 software update
• set the BOD to 2.6V (dont go higher than that)

• Added charger wake flag

• Added charger indicator

• Set the software version number to match the hardware number
</commit_message>
<xml_diff>
--- a/Hardware/Complete v3.0/Complete v2.0 Component Review.xlsx
+++ b/Hardware/Complete v3.0/Complete v2.0 Component Review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pyka\Documents\GitHub\Sonar-Watch\Hardware\Complete v2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pyka\Documents\GitHub\Sonar-Watch\Hardware\Complete v3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE12788-0FBF-48C0-BA4B-360BE35CA765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C1EF46-C24C-427A-8462-92544A2E32D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3675" yWindow="0" windowWidth="28800" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Connections" sheetId="1" r:id="rId1"/>
@@ -1394,7 +1394,7 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1451,7 +1451,6 @@
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1464,16 +1463,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1494,31 +1486,19 @@
   </cellStyles>
   <dxfs count="33">
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Tahoma"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -1527,10 +1507,231 @@
         </right>
         <top/>
         <bottom/>
-        <vertical style="thin">
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
           <color auto="1"/>
-        </vertical>
-        <horizontal/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1815,19 +2016,31 @@
       </font>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -1836,231 +2049,10 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
+        <vertical style="thin">
           <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
+        </vertical>
+        <horizontal/>
       </border>
     </dxf>
   </dxfs>
@@ -2225,51 +2217,51 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F875B8B-340B-40CB-BD49-2ED660196E2B}" name="Table1" displayName="Table1" ref="B2:J22" totalsRowShown="0" headerRowDxfId="1" dataDxfId="12" headerRowBorderDxfId="0" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F875B8B-340B-40CB-BD49-2ED660196E2B}" name="Table1" displayName="Table1" ref="B2:J22" totalsRowShown="0" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29">
   <autoFilter ref="B2:J22" xr:uid="{5F875B8B-340B-40CB-BD49-2ED660196E2B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:J15">
     <sortCondition ref="B2:B15"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{63D33BDA-CDB6-406E-9542-74C72330FFE7}" name="Index" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{C11F4ED7-F654-4000-8FE5-7F7F78A9CC23}" name="Item" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{2A73A2A3-326A-46F6-B008-BC7209351DF5}" name="Added?" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{43E1388A-9A47-4270-8D95-5DAB8EEB5C98}" name="Acquired" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{ECFAD228-AFD7-4089-BBEF-3B76C8ED16D3}" name="Board Count" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{A391AA9A-2736-457B-ACEF-2AF43BD07714}" name="Purchase Amount" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{63D33BDA-CDB6-406E-9542-74C72330FFE7}" name="Index" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{C11F4ED7-F654-4000-8FE5-7F7F78A9CC23}" name="Item" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{2A73A2A3-326A-46F6-B008-BC7209351DF5}" name="Added?" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{43E1388A-9A47-4270-8D95-5DAB8EEB5C98}" name="Acquired" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{ECFAD228-AFD7-4089-BBEF-3B76C8ED16D3}" name="Board Count" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{A391AA9A-2736-457B-ACEF-2AF43BD07714}" name="Purchase Amount" dataDxfId="23">
       <calculatedColumnFormula>F3*15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{403CC425-E277-4465-8F64-A609F52AC5F9}" name="Unit Price" dataDxfId="4" dataCellStyle="Currency"/>
-    <tableColumn id="7" xr3:uid="{3EB62525-E5E4-49DC-BF5E-1E259F7C741F}" name="Max Price" dataDxfId="3" dataCellStyle="Currency">
+    <tableColumn id="6" xr3:uid="{403CC425-E277-4465-8F64-A609F52AC5F9}" name="Unit Price" dataDxfId="22" dataCellStyle="Currency"/>
+    <tableColumn id="7" xr3:uid="{3EB62525-E5E4-49DC-BF5E-1E259F7C741F}" name="Max Price" dataDxfId="21" dataCellStyle="Currency">
       <calculatedColumnFormula>H3*G3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{FC499A18-5CC0-4737-A28D-08FFE478FD5E}" name="Link" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{FC499A18-5CC0-4737-A28D-08FFE478FD5E}" name="Link" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E2005B0A-3599-403B-A9F1-67AD927B2DA7}" name="Table15" displayName="Table15" ref="B5:R206" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" tableBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E2005B0A-3599-403B-A9F1-67AD927B2DA7}" name="Table15" displayName="Table15" ref="B5:R206" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17">
   <autoFilter ref="B5:R206" xr:uid="{58264688-3865-4782-9A70-009A39C8F454}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{AA19D35E-3785-49AE-A26C-83E80E6966A2}" name="LED\NET" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{109E106D-C958-4DA9-91C3-B22ACBA9543F}" name="1" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{D86FCCE5-8AA5-4E09-9F54-321941353303}" name="2" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{B772412E-5CEF-452F-BBCE-618D0B5878B2}" name="3" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{AAA21CAE-5015-48F0-AB8F-8419D22FE09D}" name="4" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{7FFC56BC-5441-4F47-BFED-67D91DAD6D61}" name="5" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{D1079A3A-9756-42F7-9A0D-897121BE9B7D}" name="6" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{0BF0A821-D6F0-442A-BD6B-F0B195B2FA97}" name="7" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{0C192674-A6F4-4C28-9FAF-5A452D15D3B8}" name="8" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{47C85327-AED8-4B13-BCEA-63660179BFDB}" name="9" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{B2450332-8C50-4900-B7C5-9F6320F4B5D8}" name="10" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{6707C414-32E0-45E2-8B01-756DAB7C3C7F}" name="11" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{B28386EA-1923-43C5-9A52-FE182FE09C46}" name="12" dataDxfId="17"/>
-    <tableColumn id="14" xr3:uid="{4B89B083-BD25-4DF4-A2AA-D4E133541A33}" name="13" dataDxfId="16"/>
-    <tableColumn id="15" xr3:uid="{8D659A80-CB90-4404-8FD1-7C0A68E90162}" name="14" dataDxfId="15"/>
-    <tableColumn id="16" xr3:uid="{3D79F4F0-D193-4E1F-90F1-3CD1AF69EFC5}" name="15" dataDxfId="14"/>
-    <tableColumn id="17" xr3:uid="{561F49F1-969D-4863-B381-BB2535B46E93}" name="16" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{AA19D35E-3785-49AE-A26C-83E80E6966A2}" name="LED\NET" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{109E106D-C958-4DA9-91C3-B22ACBA9543F}" name="1" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{D86FCCE5-8AA5-4E09-9F54-321941353303}" name="2" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{B772412E-5CEF-452F-BBCE-618D0B5878B2}" name="3" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{AAA21CAE-5015-48F0-AB8F-8419D22FE09D}" name="4" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{7FFC56BC-5441-4F47-BFED-67D91DAD6D61}" name="5" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{D1079A3A-9756-42F7-9A0D-897121BE9B7D}" name="6" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{0BF0A821-D6F0-442A-BD6B-F0B195B2FA97}" name="7" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{0C192674-A6F4-4C28-9FAF-5A452D15D3B8}" name="8" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{47C85327-AED8-4B13-BCEA-63660179BFDB}" name="9" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{B2450332-8C50-4900-B7C5-9F6320F4B5D8}" name="10" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{6707C414-32E0-45E2-8B01-756DAB7C3C7F}" name="11" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{B28386EA-1923-43C5-9A52-FE182FE09C46}" name="12" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{4B89B083-BD25-4DF4-A2AA-D4E133541A33}" name="13" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{8D659A80-CB90-4404-8FD1-7C0A68E90162}" name="14" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{3D79F4F0-D193-4E1F-90F1-3CD1AF69EFC5}" name="15" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{561F49F1-969D-4863-B381-BB2535B46E93}" name="16" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3877,7 +3869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B90A0B9-1C04-4F19-B584-C2078B6C916A}">
   <dimension ref="B2:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
@@ -3890,664 +3882,664 @@
     <col min="5" max="5" width="16.140625" style="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" style="21" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="19.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="19.42578125" style="22" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" style="21" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="32" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="24">
+      <c r="B3" s="23">
         <v>1</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3" s="24">
         <f>COUNTIF(Connections!C:C,Parts!C3)</f>
         <v>0</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="24">
         <f t="shared" ref="G3:G16" si="0">F3*15</f>
         <v>0</v>
       </c>
-      <c r="H3" s="26">
+      <c r="H3" s="25">
         <v>0.24</v>
       </c>
-      <c r="I3" s="26">
+      <c r="I3" s="25">
         <f t="shared" ref="I3:I16" si="1">H3*G3</f>
         <v>0</v>
       </c>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="26" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <v>2</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="24">
         <f>COUNTIF(Connections!C:C,Parts!C4)</f>
         <v>0</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H4" s="26">
+      <c r="H4" s="25">
         <v>0.21</v>
       </c>
-      <c r="I4" s="26">
+      <c r="I4" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J4" s="27" t="s">
+      <c r="J4" s="26" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="24">
+      <c r="B5" s="23">
         <v>3</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="24">
         <f>COUNTIF(Connections!C:C,Parts!C5)</f>
         <v>1</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="24">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H5" s="26">
+      <c r="H5" s="25">
         <v>0.76</v>
       </c>
-      <c r="I5" s="26">
+      <c r="I5" s="25">
         <f t="shared" si="1"/>
         <v>11.4</v>
       </c>
-      <c r="J5" s="28" t="s">
+      <c r="J5" s="27" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="24">
+      <c r="B6" s="23">
         <v>4</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="24">
         <f>COUNTIF(Connections!C:C,Parts!C6)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H6" s="25">
         <f>13.29/10</f>
         <v>1.329</v>
       </c>
-      <c r="I6" s="26">
+      <c r="I6" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J6" s="28" t="s">
+      <c r="J6" s="27" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="24">
+      <c r="B7" s="23">
         <v>5</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="24">
         <f>COUNTIF(Connections!C:C,Parts!C7)</f>
         <v>0</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H7" s="26">
+      <c r="H7" s="25">
         <v>1.3</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J7" s="28" t="s">
+      <c r="J7" s="27" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="24">
+      <c r="B8" s="23">
         <v>6</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="24">
         <f>COUNTIF(Connections!C:C,Parts!C8)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="26">
+      <c r="H8" s="25">
         <v>0.36</v>
       </c>
-      <c r="I8" s="26">
+      <c r="I8" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J8" s="28" t="s">
+      <c r="J8" s="27" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="24">
+      <c r="B9" s="23">
         <v>8</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="24">
         <f>COUNTIF(Connections!C:C,Parts!C9)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H9" s="26">
+      <c r="H9" s="25">
         <v>0.56999999999999995</v>
       </c>
-      <c r="I9" s="26">
+      <c r="I9" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J9" s="28" t="s">
+      <c r="J9" s="27" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="24">
+      <c r="B10" s="23">
         <v>9</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25" t="s">
+      <c r="D10" s="24"/>
+      <c r="E10" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="24">
         <f>COUNTIF(Connections!C:C,Parts!C10)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="26">
+      <c r="H10" s="25">
         <v>4.87</v>
       </c>
-      <c r="I10" s="26">
+      <c r="I10" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J10" s="28" t="s">
+      <c r="J10" s="27" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="24">
+      <c r="B11" s="23">
         <v>10</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="24">
         <f>COUNTIF(Connections!C:C,Parts!C11)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11" s="26">
+      <c r="H11" s="25">
         <v>0.1</v>
       </c>
-      <c r="I11" s="26">
+      <c r="I11" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J11" s="28" t="s">
+      <c r="J11" s="27" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="24">
+      <c r="B12" s="23">
         <v>11</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="24">
         <f>COUNTIF(Connections!C:C,Parts!C12)</f>
         <v>0</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="26">
+      <c r="H12" s="25">
         <v>0.1</v>
       </c>
-      <c r="I12" s="26">
+      <c r="I12" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J12" s="28" t="s">
+      <c r="J12" s="27" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="24">
+      <c r="B13" s="23">
         <v>12</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="24">
         <f>COUNTIF(Connections!C:C,Parts!C13)</f>
         <v>0</v>
       </c>
-      <c r="G13" s="25">
+      <c r="G13" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H13" s="26">
+      <c r="H13" s="25">
         <v>0.1</v>
       </c>
-      <c r="I13" s="26">
+      <c r="I13" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="28" t="s">
+      <c r="J13" s="27" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="24">
+      <c r="B14" s="23">
         <v>13</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="24">
         <v>1</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="24">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H14" s="26">
+      <c r="H14" s="25">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I14" s="26">
+      <c r="I14" s="25">
         <f t="shared" si="1"/>
         <v>4.2</v>
       </c>
-      <c r="J14" s="28" t="s">
+      <c r="J14" s="27" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="24">
+      <c r="B15" s="23">
         <v>14</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15" s="24">
         <v>1</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="24">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H15" s="26">
+      <c r="H15" s="25">
         <f>9.99/2</f>
         <v>4.9950000000000001</v>
       </c>
-      <c r="I15" s="26">
+      <c r="I15" s="25">
         <f t="shared" si="1"/>
         <v>74.924999999999997</v>
       </c>
-      <c r="J15" s="28" t="s">
+      <c r="J15" s="27" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="24">
+      <c r="B16" s="23">
         <v>15</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="24">
         <v>1</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16" s="24">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H16" s="26">
+      <c r="H16" s="25">
         <v>0.1</v>
       </c>
-      <c r="I16" s="26">
+      <c r="I16" s="25">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="J16" s="28" t="s">
+      <c r="J16" s="27" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="24">
+      <c r="B17" s="23">
         <v>16</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="24">
         <v>1</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17" s="24">
         <v>3</v>
       </c>
-      <c r="H17" s="26">
+      <c r="H17" s="25">
         <v>11.41</v>
       </c>
-      <c r="I17" s="26">
+      <c r="I17" s="25">
         <f t="shared" ref="I17:I18" si="2">H17*G17</f>
         <v>34.230000000000004</v>
       </c>
-      <c r="J17" s="28" t="s">
+      <c r="J17" s="27" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="2:10" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="29">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="23">
         <v>17</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="E18" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="30">
+      <c r="F18" s="24">
         <v>1</v>
       </c>
-      <c r="G18" s="30">
+      <c r="G18" s="24">
         <f t="shared" ref="G18" si="3">F18*15</f>
         <v>15</v>
       </c>
-      <c r="H18" s="31">
+      <c r="H18" s="28">
         <v>0.4</v>
       </c>
-      <c r="I18" s="31">
+      <c r="I18" s="28">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="J18" s="32" t="s">
+      <c r="J18" s="27" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="24">
+      <c r="B19" s="23">
         <v>18</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="E19" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="25">
+      <c r="F19" s="24">
         <v>201</v>
       </c>
-      <c r="G19" s="25">
+      <c r="G19" s="24">
         <v>500</v>
       </c>
-      <c r="H19" s="26">
+      <c r="H19" s="25">
         <v>33.340000000000003</v>
       </c>
-      <c r="I19" s="26">
+      <c r="I19" s="25">
         <f>H19</f>
         <v>33.340000000000003</v>
       </c>
-      <c r="J19" s="28" t="s">
+      <c r="J19" s="27" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B20" s="24">
+      <c r="B20" s="23">
         <v>18</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="E20" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20" s="24">
         <v>2</v>
       </c>
-      <c r="G20" s="25">
+      <c r="G20" s="24">
         <f t="shared" ref="G20" si="4">F20*15</f>
         <v>30</v>
       </c>
-      <c r="H20" s="26">
+      <c r="H20" s="25">
         <v>0.1</v>
       </c>
-      <c r="I20" s="26">
+      <c r="I20" s="25">
         <f t="shared" ref="I20:I21" si="5">H20*G20</f>
         <v>3</v>
       </c>
-      <c r="J20" s="28" t="s">
+      <c r="J20" s="27" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="24">
+      <c r="B21" s="23">
         <v>19</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="25" t="s">
+      <c r="E21" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="25">
+      <c r="F21" s="24">
         <v>1</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21" s="24">
         <v>10</v>
       </c>
-      <c r="H21" s="26">
+      <c r="H21" s="25">
         <v>1.57</v>
       </c>
-      <c r="I21" s="26">
+      <c r="I21" s="25">
         <f t="shared" si="5"/>
         <v>15.700000000000001</v>
       </c>
-      <c r="J21" s="28" t="s">
+      <c r="J21" s="27" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="24">
+      <c r="B22" s="23">
         <v>20</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="24" t="s">
         <v>383</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22" s="24">
         <v>1</v>
       </c>
-      <c r="G22" s="25">
+      <c r="G22" s="24">
         <v>100</v>
       </c>
-      <c r="H22" s="26">
+      <c r="H22" s="25">
         <v>6.95</v>
       </c>
-      <c r="I22" s="26">
+      <c r="I22" s="25">
         <f>Table1[[#This Row],[Unit Price]]</f>
         <v>6.95</v>
       </c>
-      <c r="J22" s="28" t="s">
+      <c r="J22" s="27" t="s">
         <v>384</v>
       </c>
     </row>
@@ -4568,8 +4560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0D8094C-BAC7-4D03-81AB-DB1439CDC67D}">
   <dimension ref="B2:L44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4671,6 +4663,10 @@
       </c>
       <c r="D13" s="2" t="s">
         <v>18</v>
+      </c>
+      <c r="F13">
+        <f>40/C13</f>
+        <v>4000</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Last Update - Part 1
Well, this project is coming to an end. I have found a way to safely shut down the watch - by checking the battery voltage by intervals of seconds * previous battery percentage. That way, 99% will have the battery checked 99 seconds (max charge == safe) and   1% is every second (lowest charge == danger). This ensures a safe shut down
</commit_message>
<xml_diff>
--- a/Hardware/Complete v3.0/Complete v2.0 Component Review.xlsx
+++ b/Hardware/Complete v3.0/Complete v2.0 Component Review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pyka\Documents\GitHub\Sonar-Watch\Hardware\Complete v3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C1EF46-C24C-427A-8462-92544A2E32D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC251FF-87D0-4E71-804D-337FB4838FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3675" yWindow="0" windowWidth="28800" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Connections" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="391">
   <si>
     <t>A</t>
   </si>
@@ -1182,24 +1182,44 @@
     <t>Pin</t>
   </si>
   <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Percent</t>
-  </si>
-  <si>
     <t>SI2301DS</t>
   </si>
   <si>
     <t>https://www.amazon.com/dp/B08RHQGB8F?ref=ppx_yo2ov_dt_b_fed_asin_title</t>
+  </si>
+  <si>
+    <t>Voltage Ladder Part 4 - Finding minum voltage to portect battery</t>
+  </si>
+  <si>
+    <t>Voltage - capacity chart</t>
+  </si>
+  <si>
+    <t>Raw data</t>
+  </si>
+  <si>
+    <t>Cap</t>
+  </si>
+  <si>
+    <t>Scaled volts</t>
+  </si>
+  <si>
+    <t>inverse charge</t>
+  </si>
+  <si>
+    <t>adjsuted volts</t>
+  </si>
+  <si>
+    <t>Needed data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -1394,7 +1414,7 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1448,8 +1468,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1478,6 +1496,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -2070,6 +2094,969 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Math!$K$45:$K$68</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>4.1444490856944602</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0994927776762502</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0545364696580304</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0218713520085601</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9687748716093401</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.9279486959537802</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.8625923536234601</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.8258806461117301</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.79330951377518</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.74845241247617</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.72815158488328</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.7078820857280301</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.69583108004788</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.66744229413673</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.66769292163788</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.6638395238077401</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.6518355107840601</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.6110772134100602</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.5661887836733999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.5172276570431098</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.3904414699004501</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.2677332010577</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.12864538073375</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.9895471175972501</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Math!$L$45:$L$68</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0.28866917542809101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.42661127003251</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5645533646369199</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.0099616972553997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.5245648517307</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.734387062847</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.859894751367801</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.682411692966301</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26.8829323417634</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31.9290485478896</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>36.824788253327696</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42.638898730825296</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>49.372275078600801</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>57.175293797342199</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>64.522259973818294</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>71.562655010498702</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>79.673587516363497</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>84.8732130669421</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>89.000958501008796</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>93.740503567339303</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>97.093989042505996</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>99.988736680751998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>102.72863232721799</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>105.162404382997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5724-489F-B5A1-5E59237A017F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="799680304"/>
+        <c:axId val="799678384"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="799680304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="799678384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="799678384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="799680304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -2081,7 +3068,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>189558</xdr:colOff>
+      <xdr:colOff>151458</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>27831</xdr:rowOff>
     </xdr:to>
@@ -2118,15 +3105,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>342324</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>151881</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2211,6 +3198,86 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>503770</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>115711</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>65264</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>151345</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{343F10F0-9724-D507-AC7D-525F472544B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="9658350" y="7306031"/>
+          <a:ext cx="4036134" cy="2609494"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FA1FCA0-C671-2296-76B0-EA3BCF27A853}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3875,672 +4942,672 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="21"/>
-    <col min="2" max="2" width="12.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="19.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="21" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="21"/>
+    <col min="1" max="1" width="9.140625" style="19"/>
+    <col min="2" max="2" width="12.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="19.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="19" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="30" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="23">
+      <c r="B3" s="21">
         <v>1</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="22">
         <f>COUNTIF(Connections!C:C,Parts!C3)</f>
         <v>0</v>
       </c>
-      <c r="G3" s="24">
+      <c r="G3" s="22">
         <f t="shared" ref="G3:G16" si="0">F3*15</f>
         <v>0</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H3" s="23">
         <v>0.24</v>
       </c>
-      <c r="I3" s="25">
+      <c r="I3" s="23">
         <f t="shared" ref="I3:I16" si="1">H3*G3</f>
         <v>0</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="24" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="23">
+      <c r="B4" s="21">
         <v>2</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="22">
         <f>COUNTIF(Connections!C:C,Parts!C4)</f>
         <v>0</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="23">
         <v>0.21</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J4" s="26" t="s">
+      <c r="J4" s="24" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="23">
+      <c r="B5" s="21">
         <v>3</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="22">
         <f>COUNTIF(Connections!C:C,Parts!C5)</f>
         <v>1</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="22">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="23">
         <v>0.76</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="23">
         <f t="shared" si="1"/>
         <v>11.4</v>
       </c>
-      <c r="J5" s="27" t="s">
+      <c r="J5" s="25" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="23">
+      <c r="B6" s="21">
         <v>4</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="22">
         <f>COUNTIF(Connections!C:C,Parts!C6)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G6" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="23">
         <f>13.29/10</f>
         <v>1.329</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J6" s="27" t="s">
+      <c r="J6" s="25" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="23">
+      <c r="B7" s="21">
         <v>5</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="22">
         <f>COUNTIF(Connections!C:C,Parts!C7)</f>
         <v>0</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="23">
         <v>1.3</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J7" s="27" t="s">
+      <c r="J7" s="25" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="23">
+      <c r="B8" s="21">
         <v>6</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="22">
         <f>COUNTIF(Connections!C:C,Parts!C8)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="23">
         <v>0.36</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I8" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J8" s="27" t="s">
+      <c r="J8" s="25" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="23">
+      <c r="B9" s="21">
         <v>8</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="22">
         <f>COUNTIF(Connections!C:C,Parts!C9)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="23">
         <v>0.56999999999999995</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J9" s="27" t="s">
+      <c r="J9" s="25" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="23">
+      <c r="B10" s="21">
         <v>9</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24" t="s">
+      <c r="D10" s="22"/>
+      <c r="E10" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="22">
         <f>COUNTIF(Connections!C:C,Parts!C10)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="23">
         <v>4.87</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J10" s="27" t="s">
+      <c r="J10" s="25" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="23">
+      <c r="B11" s="21">
         <v>10</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="24">
+      <c r="F11" s="22">
         <f>COUNTIF(Connections!C:C,Parts!C11)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G11" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11" s="25">
+      <c r="H11" s="23">
         <v>0.1</v>
       </c>
-      <c r="I11" s="25">
+      <c r="I11" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J11" s="27" t="s">
+      <c r="J11" s="25" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="23">
+      <c r="B12" s="21">
         <v>11</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="24">
+      <c r="F12" s="22">
         <f>COUNTIF(Connections!C:C,Parts!C12)</f>
         <v>0</v>
       </c>
-      <c r="G12" s="24">
+      <c r="G12" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H12" s="23">
         <v>0.1</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J12" s="27" t="s">
+      <c r="J12" s="25" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="23">
+      <c r="B13" s="21">
         <v>12</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="24">
+      <c r="F13" s="22">
         <f>COUNTIF(Connections!C:C,Parts!C13)</f>
         <v>0</v>
       </c>
-      <c r="G13" s="24">
+      <c r="G13" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H13" s="25">
+      <c r="H13" s="23">
         <v>0.1</v>
       </c>
-      <c r="I13" s="25">
+      <c r="I13" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="27" t="s">
+      <c r="J13" s="25" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="23">
+      <c r="B14" s="21">
         <v>13</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="24">
+      <c r="F14" s="22">
         <v>1</v>
       </c>
-      <c r="G14" s="24">
+      <c r="G14" s="22">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H14" s="23">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I14" s="23">
         <f t="shared" si="1"/>
         <v>4.2</v>
       </c>
-      <c r="J14" s="27" t="s">
+      <c r="J14" s="25" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="23">
+      <c r="B15" s="21">
         <v>14</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="24">
+      <c r="F15" s="22">
         <v>1</v>
       </c>
-      <c r="G15" s="24">
+      <c r="G15" s="22">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H15" s="23">
         <f>9.99/2</f>
         <v>4.9950000000000001</v>
       </c>
-      <c r="I15" s="25">
+      <c r="I15" s="23">
         <f t="shared" si="1"/>
         <v>74.924999999999997</v>
       </c>
-      <c r="J15" s="27" t="s">
+      <c r="J15" s="25" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="23">
+      <c r="B16" s="21">
         <v>15</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="24">
+      <c r="F16" s="22">
         <v>1</v>
       </c>
-      <c r="G16" s="24">
+      <c r="G16" s="22">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H16" s="25">
+      <c r="H16" s="23">
         <v>0.1</v>
       </c>
-      <c r="I16" s="25">
+      <c r="I16" s="23">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="J16" s="27" t="s">
+      <c r="J16" s="25" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="23">
+      <c r="B17" s="21">
         <v>16</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="24">
+      <c r="F17" s="22">
         <v>1</v>
       </c>
-      <c r="G17" s="24">
+      <c r="G17" s="22">
         <v>3</v>
       </c>
-      <c r="H17" s="25">
+      <c r="H17" s="23">
         <v>11.41</v>
       </c>
-      <c r="I17" s="25">
+      <c r="I17" s="23">
         <f t="shared" ref="I17:I18" si="2">H17*G17</f>
         <v>34.230000000000004</v>
       </c>
-      <c r="J17" s="27" t="s">
+      <c r="J17" s="25" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="23">
+      <c r="B18" s="21">
         <v>17</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="D18" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="24">
+      <c r="F18" s="22">
         <v>1</v>
       </c>
-      <c r="G18" s="24">
+      <c r="G18" s="22">
         <f t="shared" ref="G18" si="3">F18*15</f>
         <v>15</v>
       </c>
-      <c r="H18" s="28">
+      <c r="H18" s="26">
         <v>0.4</v>
       </c>
-      <c r="I18" s="28">
+      <c r="I18" s="26">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="J18" s="27" t="s">
+      <c r="J18" s="25" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="23">
+      <c r="B19" s="21">
         <v>18</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="D19" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="24">
+      <c r="F19" s="22">
         <v>201</v>
       </c>
-      <c r="G19" s="24">
+      <c r="G19" s="22">
         <v>500</v>
       </c>
-      <c r="H19" s="25">
+      <c r="H19" s="23">
         <v>33.340000000000003</v>
       </c>
-      <c r="I19" s="25">
+      <c r="I19" s="23">
         <f>H19</f>
         <v>33.340000000000003</v>
       </c>
-      <c r="J19" s="27" t="s">
+      <c r="J19" s="25" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B20" s="23">
+      <c r="B20" s="21">
         <v>18</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="24">
+      <c r="F20" s="22">
         <v>2</v>
       </c>
-      <c r="G20" s="24">
+      <c r="G20" s="22">
         <f t="shared" ref="G20" si="4">F20*15</f>
         <v>30</v>
       </c>
-      <c r="H20" s="25">
+      <c r="H20" s="23">
         <v>0.1</v>
       </c>
-      <c r="I20" s="25">
+      <c r="I20" s="23">
         <f t="shared" ref="I20:I21" si="5">H20*G20</f>
         <v>3</v>
       </c>
-      <c r="J20" s="27" t="s">
+      <c r="J20" s="25" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="23">
+      <c r="B21" s="21">
         <v>19</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="D21" s="24" t="s">
+      <c r="D21" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="24">
+      <c r="F21" s="22">
         <v>1</v>
       </c>
-      <c r="G21" s="24">
+      <c r="G21" s="22">
         <v>10</v>
       </c>
-      <c r="H21" s="25">
+      <c r="H21" s="23">
         <v>1.57</v>
       </c>
-      <c r="I21" s="25">
+      <c r="I21" s="23">
         <f t="shared" si="5"/>
         <v>15.700000000000001</v>
       </c>
-      <c r="J21" s="27" t="s">
+      <c r="J21" s="25" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="23">
+      <c r="B22" s="21">
         <v>20</v>
       </c>
-      <c r="C22" s="24" t="s">
-        <v>383</v>
-      </c>
-      <c r="D22" s="24" t="s">
+      <c r="C22" s="22" t="s">
+        <v>381</v>
+      </c>
+      <c r="D22" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="24" t="s">
+      <c r="E22" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="24">
+      <c r="F22" s="22">
         <v>1</v>
       </c>
-      <c r="G22" s="24">
+      <c r="G22" s="22">
         <v>100</v>
       </c>
-      <c r="H22" s="25">
+      <c r="H22" s="23">
         <v>6.95</v>
       </c>
-      <c r="I22" s="25">
+      <c r="I22" s="23">
         <f>Table1[[#This Row],[Unit Price]]</f>
         <v>6.95</v>
       </c>
-      <c r="J22" s="27" t="s">
-        <v>384</v>
+      <c r="J22" s="25" t="s">
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -4558,26 +5625,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0D8094C-BAC7-4D03-81AB-DB1439CDC67D}">
-  <dimension ref="B2:L44"/>
+  <dimension ref="B2:Z68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>38</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="Z2" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>39</v>
       </c>
@@ -4588,7 +5660,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
@@ -4600,7 +5672,7 @@
       </c>
       <c r="E4" s="10"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
@@ -4615,7 +5687,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
@@ -4626,7 +5698,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>19</v>
       </c>
@@ -4638,12 +5710,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>39</v>
       </c>
@@ -4654,11 +5726,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="31">
         <v>0.01</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -4669,7 +5741,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>47</v>
       </c>
@@ -4681,7 +5753,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>44</v>
       </c>
@@ -4692,7 +5764,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>45</v>
       </c>
@@ -4760,7 +5832,7 @@
       </c>
       <c r="C23" s="2">
         <f>C27/C24</f>
-        <v>6.6666666666666671E-3</v>
+        <v>7.1428571428571426E-3</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>18</v>
@@ -4772,7 +5844,7 @@
       </c>
       <c r="C24" s="2">
         <f>SUM(C25:C26)</f>
-        <v>450</v>
+        <v>420</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>43</v>
@@ -4794,7 +5866,7 @@
         <v>11</v>
       </c>
       <c r="C26" s="2">
-        <v>330</v>
+        <v>300</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>43</v>
@@ -4817,7 +5889,7 @@
       </c>
       <c r="C28" s="2">
         <f>C27-C23*C25</f>
-        <v>2.2000000000000002</v>
+        <v>2.1428571428571428</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>37</v>
@@ -4850,31 +5922,31 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C33" s="2">
         <f>C37/C34</f>
-        <v>9.3555555555555562E-3</v>
+        <v>7.3809523809523813E-3</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C34" s="2">
         <f>SUM(C35:C36)</f>
-        <v>450</v>
+        <v>420</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>32</v>
       </c>
@@ -4885,32 +5957,32 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C36" s="2">
-        <v>330</v>
+        <v>300</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L36" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M36" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C37" s="2">
-        <v>4.21</v>
+        <v>3.1</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>2</v>
       </c>
@@ -4921,48 +5993,566 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>45</v>
       </c>
       <c r="C39" s="14">
         <f>C37-C35*C33</f>
-        <v>3.0873333333333335</v>
+        <v>2.2142857142857144</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E41" s="7" t="s">
-        <v>381</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E42" s="19">
-        <v>0.97222222222222221</v>
-      </c>
-      <c r="F42">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E43" s="20">
-        <v>0.52847222222222223</v>
-      </c>
-      <c r="F43">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E44" s="20">
-        <v>4.6527777777777779E-2</v>
-      </c>
-      <c r="F44">
-        <v>80</v>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B41" s="7" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" s="2">
+        <f>C47/C44</f>
+        <v>7.619047619047619E-3</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K43" t="s">
+        <v>385</v>
+      </c>
+      <c r="N43" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B44" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="2">
+        <f>SUM(C45:C46)</f>
+        <v>420</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K44" t="s">
+        <v>37</v>
+      </c>
+      <c r="L44" t="s">
+        <v>386</v>
+      </c>
+      <c r="N44" t="s">
+        <v>389</v>
+      </c>
+      <c r="O44" t="s">
+        <v>387</v>
+      </c>
+      <c r="P44" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45" s="2">
+        <v>120</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K45" s="33">
+        <v>4.1444490856944602</v>
+      </c>
+      <c r="L45" s="33">
+        <v>0.28866917542809101</v>
+      </c>
+      <c r="N45">
+        <v>4.2</v>
+      </c>
+      <c r="O45" s="32">
+        <f>N45 - $C$45*(N45/$C$44)</f>
+        <v>3</v>
+      </c>
+      <c r="P45" s="34">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B46" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="2">
+        <v>300</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K46" s="33">
+        <v>4.0994927776762502</v>
+      </c>
+      <c r="L46" s="33">
+        <v>2.42661127003251</v>
+      </c>
+      <c r="N46" s="33">
+        <v>4.1444490856944602</v>
+      </c>
+      <c r="O46" s="32">
+        <f>N46 - $C$45*(N46/$C$44)</f>
+        <v>2.9603207754960428</v>
+      </c>
+      <c r="P46" s="34">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B47" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K47" s="33">
+        <v>4.0545364696580304</v>
+      </c>
+      <c r="L47" s="33">
+        <v>4.5645533646369199</v>
+      </c>
+      <c r="N47" s="33">
+        <v>4.0994927776762502</v>
+      </c>
+      <c r="O47" s="32">
+        <f>N47 - $C$45*(N47/$C$44)</f>
+        <v>2.9282091269116073</v>
+      </c>
+      <c r="P47" s="34">
+        <f>100-L46</f>
+        <v>97.57338872996749</v>
+      </c>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K48" s="33">
+        <v>4.0218713520085601</v>
+      </c>
+      <c r="L48" s="33">
+        <v>7.0099616972553997</v>
+      </c>
+      <c r="N48" s="33">
+        <v>4.0545364696580304</v>
+      </c>
+      <c r="O48" s="32">
+        <f>N48 - $C$45*(N48/$C$44)</f>
+        <v>2.8960974783271647</v>
+      </c>
+      <c r="P48" s="34">
+        <f>100-L47</f>
+        <v>95.435446635363078</v>
+      </c>
+    </row>
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" s="14">
+        <f>C47-C45*C43</f>
+        <v>2.285714285714286</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K49" s="33">
+        <v>3.9687748716093401</v>
+      </c>
+      <c r="L49" s="33">
+        <v>10.5245648517307</v>
+      </c>
+      <c r="N49" s="33">
+        <v>4.0218713520085601</v>
+      </c>
+      <c r="O49" s="32">
+        <f>N49 - $C$45*(N49/$C$44)</f>
+        <v>2.8727652514346858</v>
+      </c>
+      <c r="P49" s="34">
+        <f>100-L48</f>
+        <v>92.990038302744594</v>
+      </c>
+    </row>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K50" s="33">
+        <v>3.9279486959537802</v>
+      </c>
+      <c r="L50" s="33">
+        <v>13.734387062847</v>
+      </c>
+      <c r="N50" s="33">
+        <v>3.9687748716093401</v>
+      </c>
+      <c r="O50" s="32">
+        <f>N50 - $C$45*(N50/$C$44)</f>
+        <v>2.8348391940066717</v>
+      </c>
+      <c r="P50" s="34">
+        <f>100-L49</f>
+        <v>89.475435148269298</v>
+      </c>
+    </row>
+    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K51" s="33">
+        <v>3.8625923536234601</v>
+      </c>
+      <c r="L51" s="33">
+        <v>17.859894751367801</v>
+      </c>
+      <c r="N51" s="33">
+        <v>3.9279486959537802</v>
+      </c>
+      <c r="O51" s="32">
+        <f>N51 - $C$45*(N51/$C$44)</f>
+        <v>2.8056776399669858</v>
+      </c>
+      <c r="P51" s="34">
+        <f>100-L50</f>
+        <v>86.265612937152994</v>
+      </c>
+    </row>
+    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K52" s="33">
+        <v>3.8258806461117301</v>
+      </c>
+      <c r="L52" s="33">
+        <v>21.682411692966301</v>
+      </c>
+      <c r="N52" s="33">
+        <v>3.8625923536234601</v>
+      </c>
+      <c r="O52" s="32">
+        <f>N52 - $C$45*(N52/$C$44)</f>
+        <v>2.7589945383024714</v>
+      </c>
+      <c r="P52" s="34">
+        <f>100-L51</f>
+        <v>82.140105248632196</v>
+      </c>
+    </row>
+    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K53" s="33">
+        <v>3.79330951377518</v>
+      </c>
+      <c r="L53" s="33">
+        <v>26.8829323417634</v>
+      </c>
+      <c r="N53" s="33">
+        <v>3.8258806461117301</v>
+      </c>
+      <c r="O53" s="32">
+        <f>N53 - $C$45*(N53/$C$44)</f>
+        <v>2.7327718900798073</v>
+      </c>
+      <c r="P53" s="34">
+        <f>100-L52</f>
+        <v>78.317588307033702</v>
+      </c>
+    </row>
+    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K54" s="33">
+        <v>3.74845241247617</v>
+      </c>
+      <c r="L54" s="33">
+        <v>31.9290485478896</v>
+      </c>
+      <c r="N54" s="33">
+        <v>3.79330951377518</v>
+      </c>
+      <c r="O54" s="32">
+        <f>N54 - $C$45*(N54/$C$44)</f>
+        <v>2.7095067955537</v>
+      </c>
+      <c r="P54" s="34">
+        <f>100-L53</f>
+        <v>73.117067658236607</v>
+      </c>
+    </row>
+    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K55" s="33">
+        <v>3.72815158488328</v>
+      </c>
+      <c r="L55" s="33">
+        <v>36.824788253327696</v>
+      </c>
+      <c r="N55" s="33">
+        <v>3.74845241247617</v>
+      </c>
+      <c r="O55" s="32">
+        <f>N55 - $C$45*(N55/$C$44)</f>
+        <v>2.6774660089115501</v>
+      </c>
+      <c r="P55" s="34">
+        <f>100-L54</f>
+        <v>68.070951452110393</v>
+      </c>
+    </row>
+    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K56" s="33">
+        <v>3.7078820857280301</v>
+      </c>
+      <c r="L56" s="33">
+        <v>42.638898730825296</v>
+      </c>
+      <c r="N56" s="33">
+        <v>3.72815158488328</v>
+      </c>
+      <c r="O56" s="32">
+        <f>N56 - $C$45*(N56/$C$44)</f>
+        <v>2.6629654177737714</v>
+      </c>
+      <c r="P56" s="34">
+        <f>100-L55</f>
+        <v>63.175211746672304</v>
+      </c>
+    </row>
+    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K57" s="33">
+        <v>3.69583108004788</v>
+      </c>
+      <c r="L57" s="33">
+        <v>49.372275078600801</v>
+      </c>
+      <c r="N57" s="33">
+        <v>3.7078820857280301</v>
+      </c>
+      <c r="O57" s="32">
+        <f>N57 - $C$45*(N57/$C$44)</f>
+        <v>2.6484872040914498</v>
+      </c>
+      <c r="P57" s="34">
+        <f>100-L56</f>
+        <v>57.361101269174704</v>
+      </c>
+    </row>
+    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K58" s="33">
+        <v>3.66744229413673</v>
+      </c>
+      <c r="L58" s="33">
+        <v>57.175293797342199</v>
+      </c>
+      <c r="N58" s="33">
+        <v>3.69583108004788</v>
+      </c>
+      <c r="O58" s="32">
+        <f>N58 - $C$45*(N58/$C$44)</f>
+        <v>2.639879342891343</v>
+      </c>
+      <c r="P58" s="34">
+        <f>100-L57</f>
+        <v>50.627724921399199</v>
+      </c>
+    </row>
+    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K59" s="33">
+        <v>3.66769292163788</v>
+      </c>
+      <c r="L59" s="33">
+        <v>64.522259973818294</v>
+      </c>
+      <c r="N59" s="33">
+        <v>3.66744229413673</v>
+      </c>
+      <c r="O59" s="32">
+        <f>N59 - $C$45*(N59/$C$44)</f>
+        <v>2.619601638669093</v>
+      </c>
+      <c r="P59" s="34">
+        <f>100-L58</f>
+        <v>42.824706202657801</v>
+      </c>
+    </row>
+    <row r="60" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K60" s="33">
+        <v>3.6638395238077401</v>
+      </c>
+      <c r="L60" s="33">
+        <v>71.562655010498702</v>
+      </c>
+      <c r="N60" s="33">
+        <v>3.66769292163788</v>
+      </c>
+      <c r="O60" s="32">
+        <f>N60 - $C$45*(N60/$C$44)</f>
+        <v>2.6197806583127714</v>
+      </c>
+      <c r="P60" s="34">
+        <f>100-L59</f>
+        <v>35.477740026181706</v>
+      </c>
+    </row>
+    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K61" s="33">
+        <v>3.6518355107840601</v>
+      </c>
+      <c r="L61" s="33">
+        <v>79.673587516363497</v>
+      </c>
+      <c r="N61" s="33">
+        <v>3.6638395238077401</v>
+      </c>
+      <c r="O61" s="32">
+        <f>N61 - $C$45*(N61/$C$44)</f>
+        <v>2.617028231291243</v>
+      </c>
+      <c r="P61" s="34">
+        <f>100-L60</f>
+        <v>28.437344989501298</v>
+      </c>
+    </row>
+    <row r="62" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K62" s="33">
+        <v>3.6110772134100602</v>
+      </c>
+      <c r="L62" s="33">
+        <v>84.8732130669421</v>
+      </c>
+      <c r="N62" s="33">
+        <v>3.6518355107840601</v>
+      </c>
+      <c r="O62" s="32">
+        <f>N62 - $C$45*(N62/$C$44)</f>
+        <v>2.6084539362743286</v>
+      </c>
+      <c r="P62" s="34">
+        <f>100-L61</f>
+        <v>20.326412483636503</v>
+      </c>
+    </row>
+    <row r="63" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K63" s="33">
+        <v>3.5661887836733999</v>
+      </c>
+      <c r="L63" s="33">
+        <v>89.000958501008796</v>
+      </c>
+      <c r="N63" s="33">
+        <v>3.6110772134100602</v>
+      </c>
+      <c r="O63" s="32">
+        <f>N63 - $C$45*(N63/$C$44)</f>
+        <v>2.5793408667214717</v>
+      </c>
+      <c r="P63" s="34">
+        <f>100-L62</f>
+        <v>15.1267869330579</v>
+      </c>
+    </row>
+    <row r="64" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K64" s="33">
+        <v>3.5172276570431098</v>
+      </c>
+      <c r="L64" s="33">
+        <v>93.740503567339303</v>
+      </c>
+      <c r="N64" s="33">
+        <v>3.5661887836733999</v>
+      </c>
+      <c r="O64" s="32">
+        <f>N64 - $C$45*(N64/$C$44)</f>
+        <v>2.5472777026238571</v>
+      </c>
+      <c r="P64" s="34">
+        <f>100-L63</f>
+        <v>10.999041498991204</v>
+      </c>
+    </row>
+    <row r="65" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K65" s="33">
+        <v>3.3904414699004501</v>
+      </c>
+      <c r="L65" s="33">
+        <v>97.093989042505996</v>
+      </c>
+      <c r="N65" s="33">
+        <v>3.5172276570431098</v>
+      </c>
+      <c r="O65" s="32">
+        <f>N65 - $C$45*(N65/$C$44)</f>
+        <v>2.512305469316507</v>
+      </c>
+      <c r="P65" s="34">
+        <f>100-L64</f>
+        <v>6.259496432660697</v>
+      </c>
+    </row>
+    <row r="66" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K66" s="33">
+        <v>3.2677332010577</v>
+      </c>
+      <c r="L66" s="33">
+        <v>99.988736680751998</v>
+      </c>
+      <c r="N66" s="33">
+        <v>3.3904414699004501</v>
+      </c>
+      <c r="O66" s="32">
+        <f>N66 - $C$45*(N66/$C$44)</f>
+        <v>2.4217439070717504</v>
+      </c>
+      <c r="P66" s="34">
+        <f>100-L65</f>
+        <v>2.9060109574940043</v>
+      </c>
+    </row>
+    <row r="67" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K67" s="33">
+        <v>3.12864538073375</v>
+      </c>
+      <c r="L67" s="33">
+        <v>102.72863232721799</v>
+      </c>
+      <c r="N67" s="33">
+        <v>3.2</v>
+      </c>
+      <c r="O67" s="32">
+        <f>N67 - $C$45*(N67/$C$44)</f>
+        <v>2.285714285714286</v>
+      </c>
+      <c r="P67" s="34">
+        <f>100-L66</f>
+        <v>1.1263319248001835E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K68" s="33">
+        <v>2.9895471175972501</v>
+      </c>
+      <c r="L68" s="33">
+        <v>105.162404382997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>